<commit_message>
En son Basedriver if li kisim eklendi
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resources/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resources/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="25">
   <si>
     <t>citizenship-with-apachepoi;citizenship-create-and-delete-from-excel</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>country-multi-scenario;create-a-country-parameter-data</t>
+  </si>
+  <si>
+    <t>citizenship-with-scenario-outline;citizenship-create-and-delete-with-scenario-outline;;2</t>
+  </si>
+  <si>
+    <t>21.09.2021</t>
+  </si>
+  <si>
+    <t>26.09.2021</t>
   </si>
 </sst>
 </file>
@@ -182,7 +191,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
@@ -1030,6 +1039,314 @@
         <v>19</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>